<commit_message>
Changes in the newly created changelog file
</commit_message>
<xml_diff>
--- a/TPV_Source/TPV.xlsx
+++ b/TPV_Source/TPV.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>18-06-2017</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>29-06-2017, Thursday</t>
+  </si>
+  <si>
+    <t>02-07-2017, Sunday</t>
   </si>
   <si>
     <t>Spindel</t>
@@ -420,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,9 +432,10 @@
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,10 +448,13 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -461,10 +468,13 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -478,10 +488,13 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -495,10 +508,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -512,10 +528,13 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -529,10 +548,13 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -546,10 +568,13 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -563,10 +588,13 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -580,10 +608,13 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -596,6 +627,9 @@
       </c>
       <c r="E10">
         <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>